<commit_message>
added: fixed rates comparison
</commit_message>
<xml_diff>
--- a/Mortgage Calculator.xlsx
+++ b/Mortgage Calculator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t xml:space="preserve">Disclaimer: This is a portfolio project for demonstration only. The creator is not responsible for any error.</t>
   </si>
@@ -55,13 +55,109 @@
     <t xml:space="preserve">Monthly Payments</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Similar price range in regions of ON (until September 1</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  2022)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Total Interest Paid</t>
   </si>
   <si>
+    <t xml:space="preserve">Central region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern region</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total Annual Payment</t>
   </si>
   <si>
+    <t xml:space="preserve">Greater Toronto Area</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total Payments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southwest region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Better Fixed Mortgage Rates in ON (2022)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Butler Mortgage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nesto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scotiabank</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Source: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://wowa.ca/ontario-housing-market</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -74,7 +170,7 @@
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial Unicode MS"/>
@@ -103,6 +199,34 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -113,7 +237,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,7 +253,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFD7"/>
-        <bgColor rgb="FFEEF5DB"/>
+        <bgColor rgb="FFF6F9D4"/>
       </patternFill>
     </fill>
     <fill>
@@ -141,6 +265,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDEDCE6"/>
+        <bgColor rgb="FFEEF5DB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F9D4"/>
         <bgColor rgb="FFEEF5DB"/>
       </patternFill>
     </fill>
@@ -221,7 +351,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -295,6 +425,30 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -310,7 +464,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFEEF5DB"/>
+      <rgbColor rgb="FFF6F9D4"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -323,7 +477,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FFB8D8D0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -343,9 +497,9 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFEEF5DB"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FFB8D8D0"/>
+      <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFDBB6"/>
@@ -506,7 +660,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Main!$B$18,Main!$B$21</c:f>
+              <c:f>Main!$B$18:$B$18,Main!$B$21:$B$21</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="1"/>
                 <c:lvl>
@@ -524,15 +678,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Main!$C$18,Main!$C$21</c:f>
+              <c:f>Main!$C$18:$C$18,Main!$C$21:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2909523.32771731</c:v>
+                  <c:v>3037391.55468631</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13809523.3277174</c:v>
+                  <c:v>13937391.5546864</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -569,6 +723,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -591,10 +746,10 @@
       <xdr:rowOff>131400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>58320</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>878400</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -603,7 +758,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4708440" y="456480"/>
-        <a:ext cx="3483720" cy="1959840"/>
+        <a:ext cx="3484440" cy="1959480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -621,13 +776,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.82"/>
@@ -635,6 +790,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,7 +842,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>0.049</v>
+        <v>0.051</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>3</v>
@@ -760,7 +916,7 @@
       </c>
       <c r="C13" s="15" t="n">
         <f aca="false">C6</f>
-        <v>0.049</v>
+        <v>0.051</v>
       </c>
       <c r="D13" s="0"/>
       <c r="G13" s="9"/>
@@ -793,47 +949,180 @@
       <c r="D16" s="0"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="18" t="n">
         <f aca="false">IFERROR(PMT(C13/12,C14*12,-C11),"")</f>
-        <v>115079.361064312</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>116144.929622386</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="18" t="n">
         <f aca="false">IFERROR(-CUMIPMT(C13/12,C14*12,C11,1,C14*12,0),"")</f>
-        <v>2909523.32771731</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3037391.55468631</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="16"/>
       <c r="C19" s="17"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C20" s="18" t="n">
         <f aca="false">IFERROR(C17*12,"")</f>
-        <v>1380952.33277174</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1393739.15546864</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C21" s="18" t="n">
         <f aca="false">IFERROR(C20*C14,"")</f>
-        <v>13809523.3277174</v>
-      </c>
+        <v>13937391.5546864</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="23" t="n">
+        <v>0.0427</v>
+      </c>
+      <c r="G25" s="24" t="str">
+        <f aca="false">IF(F25&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v>&lt;= May consider this instead</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="23" t="n">
+        <v>0.0429</v>
+      </c>
+      <c r="G26" s="24" t="str">
+        <f aca="false">IF(F26&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v>&lt;= May consider this instead</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="23" t="n">
+        <v>0.0434</v>
+      </c>
+      <c r="G27" s="24" t="str">
+        <f aca="false">IF(F27&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v>&lt;= May consider this instead</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="23" t="n">
+        <v>0.0517</v>
+      </c>
+      <c r="G28" s="24" t="str">
+        <f aca="false">IF(F28&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="23" t="n">
+        <v>0.0524</v>
+      </c>
+      <c r="G29" s="24" t="str">
+        <f aca="false">IF(F29&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="23" t="n">
+        <v>0.0524</v>
+      </c>
+      <c r="G30" s="24" t="str">
+        <f aca="false">IF(F30&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="23" t="n">
+        <v>0.0554</v>
+      </c>
+      <c r="G31" s="24" t="str">
+        <f aca="false">IF(F31&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" s="23" t="n">
+        <v>0.0599</v>
+      </c>
+      <c r="G32" s="24" t="str">
+        <f aca="false">IF(F32&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E33" r:id="rId1" display="https://wowa.ca/ontario-housing-market"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -841,6 +1130,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added: major cities comparison
</commit_message>
<xml_diff>
--- a/Mortgage Calculator.xlsx
+++ b/Mortgage Calculator.xlsx
@@ -49,12 +49,6 @@
     <t xml:space="preserve">Financing %</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of Payments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monthly Payments</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -63,7 +57,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Similar price range in regions of ON (until September 1</t>
+      <t xml:space="preserve">Housing Markets of Major Cities in Ontario (until September 1</t>
     </r>
     <r>
       <rPr>
@@ -88,31 +82,37 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Toronto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ottawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Payments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamilton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly Payments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mississauga</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total Interest Paid</t>
   </si>
   <si>
-    <t xml:space="preserve">Central region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern region</t>
+    <t xml:space="preserve">Brampton</t>
   </si>
   <si>
     <t xml:space="preserve">Total Annual Payment</t>
   </si>
   <si>
-    <t xml:space="preserve">Greater Toronto Area</t>
+    <t xml:space="preserve">Better Fixed Mortgage Rates in ON (2022)</t>
   </si>
   <si>
     <t xml:space="preserve">Total Payments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southwest region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Better Fixed Mortgage Rates in ON (2022)</t>
   </si>
   <si>
     <t xml:space="preserve">Butler Mortgage</t>
@@ -164,11 +164,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-1009]#,##0.00;[RED]\-[$$-1009]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="General"/>
+    <numFmt numFmtId="168" formatCode="[$$-1009]#,##0.00;[RED]\-[$$-1009]#,##0.00"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -275,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -314,6 +315,27 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -323,6 +345,13 @@
       <right style="thin"/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -351,7 +380,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -416,11 +445,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -428,15 +485,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,11 +505,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -524,7 +597,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -683,10 +756,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3037391.55468631</c:v>
+                  <c:v>227639.604716952</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13937391.5546864</c:v>
+                  <c:v>1027639.60471695</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -740,16 +813,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>874800</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>131400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>11520</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>878400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:colOff>291960</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>106560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -757,8 +830,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4708440" y="456480"/>
-        <a:ext cx="3484440" cy="1959480"/>
+        <a:off x="4728240" y="275760"/>
+        <a:ext cx="2878200" cy="1618920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -776,10 +849,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -818,7 +891,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="n">
-        <v>11000000</v>
+        <v>900000</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>3</v>
@@ -842,7 +915,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>0.051</v>
+        <v>0.052</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>3</v>
@@ -872,7 +945,7 @@
       </c>
       <c r="C9" s="14" t="n">
         <f aca="false">VALUE(C4)</f>
-        <v>11000000</v>
+        <v>900000</v>
       </c>
       <c r="D9" s="0"/>
       <c r="G9" s="9"/>
@@ -894,7 +967,7 @@
       </c>
       <c r="C11" s="14" t="n">
         <f aca="false">IF(C9-C10&lt;0,"Can't be negative!",IF(ISBLANK(C9),"",C9-C10))</f>
-        <v>10900000</v>
+        <v>800000</v>
       </c>
       <c r="D11" s="0"/>
       <c r="G11" s="9"/>
@@ -905,23 +978,27 @@
       </c>
       <c r="C12" s="15" t="n">
         <f aca="false">IFERROR(C11/C9,"Error")</f>
-        <v>0.990909090909091</v>
+        <v>0.888888888888889</v>
       </c>
       <c r="D12" s="0"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="15" t="n">
         <f aca="false">C6</f>
-        <v>0.051</v>
+        <v>0.052</v>
       </c>
       <c r="D13" s="0"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="10" t="s">
         <v>6</v>
       </c>
@@ -930,198 +1007,227 @@
         <v>10</v>
       </c>
       <c r="D14" s="0"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
+      <c r="E14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="20" t="n">
+        <f aca="false">VALUE(1019100)</f>
+        <v>1019100</v>
+      </c>
+      <c r="G14" s="21" t="str">
+        <f aca="false">IF(C4&gt;F14,"&lt;= Do you love this place?","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="0"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="20" t="n">
+        <f aca="false">VALUE(645653)</f>
+        <v>645653</v>
+      </c>
+      <c r="G15" s="24" t="str">
+        <f aca="false">IF(C4&gt;F15,"&lt;= Do you love this place?","")</f>
+        <v>&lt;= Do you love this place?</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C16" s="14" t="n">
         <f aca="false">IF(C13*12=0,"",C14*12)</f>
         <v>120</v>
       </c>
       <c r="D16" s="0"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="20" t="n">
+        <f aca="false">VALUE(79362)</f>
+        <v>79362</v>
+      </c>
+      <c r="G16" s="21" t="str">
+        <f aca="false">IF(C4&gt;F16,"&lt;= Do you love this place?","")</f>
+        <v>&lt;= Do you love this place?</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="18" t="n">
+        <v>14</v>
+      </c>
+      <c r="C17" s="25" t="n">
         <f aca="false">IFERROR(PMT(C13/12,C14*12,-C11),"")</f>
-        <v>116144.929622386</v>
+        <v>8563.66337264126</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F17" s="20" t="n">
+        <v>1068804</v>
+      </c>
+      <c r="G17" s="24" t="str">
+        <f aca="false">IF(C4&gt;F17,"&lt;= Do you love this place?","")</f>
+        <v/>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" s="25" t="n">
         <f aca="false">IFERROR(-CUMIPMT(C13/12,C14*12,C11,1,C14*12,0),"")</f>
-        <v>3037391.55468631</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="E19" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>227639.604716952</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="20" t="n">
+        <v>1027535</v>
+      </c>
+      <c r="G18" s="24" t="str">
+        <f aca="false">IF(C4&gt;F18,"&lt;= Do you love this place?","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="C20" s="25" t="n">
         <f aca="false">IFERROR(C17*12,"")</f>
-        <v>1393739.15546864</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>102763.960471695</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="30"/>
+      <c r="G20" s="24"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" s="25" t="n">
         <f aca="false">IFERROR(C20*C14,"")</f>
-        <v>13937391.5546864</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="20" t="s">
-        <v>19</v>
+        <v>1027639.60471695</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="32" t="n">
+        <v>0.0427</v>
+      </c>
+      <c r="G21" s="21" t="str">
+        <f aca="false">IF(F21&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v>&lt;= May consider this instead</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="32" t="n">
+        <v>0.0429</v>
+      </c>
+      <c r="G22" s="21" t="str">
+        <f aca="false">IF(F22&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v>&lt;= May consider this instead</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="32" t="n">
+        <v>0.0434</v>
+      </c>
+      <c r="G23" s="21" t="str">
+        <f aca="false">IF(F23&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v>&lt;= May consider this instead</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E24" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
+      <c r="E24" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="32" t="n">
+        <v>0.0517</v>
+      </c>
+      <c r="G24" s="21" t="str">
+        <f aca="false">IF(F24&lt;$C$6,"&lt;= May consider this instead","")</f>
+        <v>&lt;= May consider this instead</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E25" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="23" t="n">
-        <v>0.0427</v>
-      </c>
-      <c r="G25" s="24" t="str">
+      <c r="E25" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="32" t="n">
+        <v>0.0524</v>
+      </c>
+      <c r="G25" s="21" t="str">
         <f aca="false">IF(F25&lt;$C$6,"&lt;= May consider this instead","")</f>
-        <v>&lt;= May consider this instead</v>
+        <v/>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="23" t="n">
-        <v>0.0429</v>
-      </c>
-      <c r="G26" s="24" t="str">
+      <c r="E26" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="32" t="n">
+        <v>0.0524</v>
+      </c>
+      <c r="G26" s="21" t="str">
         <f aca="false">IF(F26&lt;$C$6,"&lt;= May consider this instead","")</f>
-        <v>&lt;= May consider this instead</v>
+        <v/>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E27" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="23" t="n">
-        <v>0.0434</v>
-      </c>
-      <c r="G27" s="24" t="str">
+      <c r="E27" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="32" t="n">
+        <v>0.0554</v>
+      </c>
+      <c r="G27" s="21" t="str">
         <f aca="false">IF(F27&lt;$C$6,"&lt;= May consider this instead","")</f>
-        <v>&lt;= May consider this instead</v>
+        <v/>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E28" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="23" t="n">
-        <v>0.0517</v>
-      </c>
-      <c r="G28" s="24" t="str">
+      <c r="E28" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="32" t="n">
+        <v>0.0599</v>
+      </c>
+      <c r="G28" s="21" t="str">
         <f aca="false">IF(F28&lt;$C$6,"&lt;= May consider this instead","")</f>
         <v/>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="23" t="n">
-        <v>0.0524</v>
-      </c>
-      <c r="G29" s="24" t="str">
-        <f aca="false">IF(F29&lt;$C$6,"&lt;= May consider this instead","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="23" t="n">
-        <v>0.0524</v>
-      </c>
-      <c r="G30" s="24" t="str">
-        <f aca="false">IF(F30&lt;$C$6,"&lt;= May consider this instead","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E31" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F31" s="23" t="n">
-        <v>0.0554</v>
-      </c>
-      <c r="G31" s="24" t="str">
-        <f aca="false">IF(F31&lt;$C$6,"&lt;= May consider this instead","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="23" t="n">
-        <v>0.0599</v>
-      </c>
-      <c r="G32" s="24" t="str">
-        <f aca="false">IF(F32&lt;$C$6,"&lt;= May consider this instead","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="22" t="s">
+    <row r="29" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="35"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E33" r:id="rId1" display="https://wowa.ca/ontario-housing-market"/>
+    <hyperlink ref="E29" r:id="rId1" display="https://wowa.ca/ontario-housing-market"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>